<commit_message>
1) Api Test examples
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/api/ApiTestData.xlsx
+++ b/src/test/resources/testdata/api/ApiTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohd.abdul/ProjectCode/demo-ui-qa/src/test/resources/testdata/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EA9634-995C-2747-B566-A0B89A4A4CEF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DD00DE-544E-5645-BE8F-7EB2057D8CB6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="980" windowWidth="23560" windowHeight="14560" tabRatio="763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllCountriesTestData" sheetId="8" r:id="rId1"/>
     <sheet name="CountryIdTestData" sheetId="7" r:id="rId2"/>
+    <sheet name="NewCountryTestData" sheetId="9" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -115,9 +116,6 @@
             "alpha3_code": "USA"
   }
 }</t>
-  </si>
-  <si>
-    <t>TC#1_AllCounvers</t>
   </si>
   <si>
     <t>Get all countries and validate that US, DE and GB were returned in the response</t>
@@ -140,6 +138,26 @@
     "alpha3_code": "GBR"
   }
 ]</t>
+  </si>
+  <si>
+    <t>TC#1_CreateNewCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify creation new country using Post call, </t>
+  </si>
+  <si>
+    <t>name: Test Country;
+ alpha2_code: TC;
+alpha3_code: TCY</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>inputData</t>
+  </si>
+  <si>
+    <t>TC#1_AllCountries</t>
   </si>
 </sst>
 </file>
@@ -578,7 +596,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -606,16 +624,16 @@
     </row>
     <row r="2" spans="1:4" ht="128" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -628,7 +646,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -729,4 +747,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B66D4CC-B198-2549-AA3A-52FA735F49AE}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
1) Demo Api Test examples
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/api/ApiTestData.xlsx
+++ b/src/test/resources/testdata/api/ApiTestData.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohd.abdul/ProjectCode/demo-ui-qa/src/test/resources/testdata/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EA9634-995C-2747-B566-A0B89A4A4CEF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAFCE2E-B6FB-B749-A5F2-0C72C22BFEF0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="980" windowWidth="23560" windowHeight="14560" tabRatio="763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4380" yWindow="1940" windowWidth="23560" windowHeight="14560" tabRatio="763" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllCountriesTestData" sheetId="8" r:id="rId1"/>
     <sheet name="CountryIdTestData" sheetId="7" r:id="rId2"/>
+    <sheet name="NewCountryTestData" sheetId="9" r:id="rId3"/>
+    <sheet name="NewCountryTestDataNegative" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -115,9 +117,6 @@
             "alpha3_code": "USA"
   }
 }</t>
-  </si>
-  <si>
-    <t>TC#1_AllCounvers</t>
   </si>
   <si>
     <t>Get all countries and validate that US, DE and GB were returned in the response</t>
@@ -140,6 +139,63 @@
     "alpha3_code": "GBR"
   }
 ]</t>
+  </si>
+  <si>
+    <t>TC#1_CreateNewCountry</t>
+  </si>
+  <si>
+    <t>inputData</t>
+  </si>
+  <si>
+    <t>Create New Country</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>TC#1_GetAllCounties</t>
+  </si>
+  <si>
+    <t>TC#1_WithoutNameField</t>
+  </si>
+  <si>
+    <t>Create New Country without Name Field</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>inputTemplateName:POST_REQ_01;
+name:Test Country;
+alpha2_code:TC;
+alpha3_code:TCY</t>
+  </si>
+  <si>
+    <t>inputTemplateName:POST_REQ_WITHOUTNAMEFIELD;
+alpha2_code:TC;
+alpha3_code:TCY</t>
+  </si>
+  <si>
+    <t>Create New Country without alpha2_code Field</t>
+  </si>
+  <si>
+    <t>inputTemplateName:POST_REQ_WITHOUTALPHA2CODE;
+alpha2_code:TC;
+alpha3_code:TCY</t>
+  </si>
+  <si>
+    <t>TC#2_Without_alpha2_codeField</t>
+  </si>
+  <si>
+    <t>TC#2_Without_alpha3_codeField</t>
+  </si>
+  <si>
+    <t>Create New Country without alpha3_code Field</t>
+  </si>
+  <si>
+    <t>inputTemplateName:POST_REQ_WITHOUTALPHA3CODE;
+alpha2_code:TC;
+alpha3_code:TCY</t>
   </si>
 </sst>
 </file>
@@ -577,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE0A40B-AECD-E045-A7D3-6045671655A4}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -606,16 +662,16 @@
     </row>
     <row r="2" spans="1:4" ht="128" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -628,7 +684,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -729,4 +785,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119C41BC-3BB1-B64C-80F6-51EE107B1D48}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB9B011-CCF6-A140-A223-533E09EFEE5E}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>